<commit_message>
Add boating organizations map product, issue #23
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
+++ b/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>This Excel workbook is an initial enventory of educational organizations that will be shown on the Basin Entities / Education - Organization map.</t>
   </si>
@@ -154,6 +154,27 @@
   </si>
   <si>
     <t>Focus on open source software and open data</t>
+  </si>
+  <si>
+    <t>LontitudeMain</t>
+  </si>
+  <si>
+    <t>LatitudeMain</t>
+  </si>
+  <si>
+    <t>Environmental Learning Center</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>University research with community access.</t>
+  </si>
+  <si>
+    <t>River habitat education, wildlife.</t>
+  </si>
+  <si>
+    <t>https://warnercnr.colostate.edu/elc/</t>
   </si>
 </sst>
 </file>
@@ -502,7 +523,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
@@ -517,9 +538,11 @@
     <col min="6" max="6" width="6.88671875" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" customWidth="1"/>
     <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -544,8 +567,14 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -561,7 +590,7 @@
       <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>26</v>
       </c>
       <c r="G2">
@@ -571,173 +600,206 @@
         <v>40.577306999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>-105.019469</v>
+      </c>
+      <c r="H3">
+        <v>40.555596999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>-105.076491</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>40.321511000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4">
-        <v>-105.00755599999999</v>
-      </c>
-      <c r="H4">
-        <v>40.565894999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>-105.00755599999999</v>
+      </c>
+      <c r="H5">
+        <v>40.565894999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>-104.812639</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>40.441882999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>-104.597244</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>40.421965999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7">
-        <v>-104.575237</v>
-      </c>
-      <c r="H7">
-        <v>40.419888999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8">
+        <v>-104.575237</v>
+      </c>
+      <c r="H8">
+        <v>40.419888999999998</v>
+      </c>
+      <c r="I8">
+        <v>-104.972905</v>
+      </c>
+      <c r="J8">
+        <v>39.742072999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>-105.07213299999999</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>40.596778</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
     <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E3" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add example for docPath for layer, issue #35
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
+++ b/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>This Excel workbook is an initial enventory of educational organizations that will be shown on the Basin Entities / Education - Organization map.</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Open Water Foundation</t>
   </si>
   <si>
-    <t>Waer data and tools for education</t>
-  </si>
-  <si>
     <t>Focus on open source software and open data</t>
   </si>
   <si>
@@ -175,6 +172,36 @@
   </si>
   <si>
     <t>https://warnercnr.colostate.edu/elc/</t>
+  </si>
+  <si>
+    <t>Water data and tools for education</t>
+  </si>
+  <si>
+    <t>West Greeley Conservation District</t>
+  </si>
+  <si>
+    <t>Water conservation</t>
+  </si>
+  <si>
+    <t>Gardens on Spring Creek</t>
+  </si>
+  <si>
+    <t>Community garden</t>
+  </si>
+  <si>
+    <t>Botanical garden with educational events</t>
+  </si>
+  <si>
+    <t>https://www.fcgov.com/gardens/</t>
+  </si>
+  <si>
+    <t>Houston Gardens</t>
+  </si>
+  <si>
+    <t>https://www.wgcd.org/houston-gardens/</t>
+  </si>
+  <si>
+    <t>https://www.wgcd.org/conservation-education/</t>
   </si>
 </sst>
 </file>
@@ -523,15 +550,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" width="36.21875" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="4" width="59.109375" customWidth="1"/>
     <col min="5" max="5" width="61.6640625" customWidth="1"/>
@@ -568,10 +596,10 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
         <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -602,19 +630,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -628,178 +656,258 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
       </c>
       <c r="G4">
-        <v>-105.076491</v>
+        <v>-105.08512899999999</v>
       </c>
       <c r="H4">
-        <v>40.321511000000001</v>
+        <v>40.561815000000003</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
       <c r="G5">
-        <v>-105.00755599999999</v>
+        <v>-104.71683400000001</v>
       </c>
       <c r="H5">
-        <v>40.565894999999998</v>
+        <v>40.428258</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
       </c>
       <c r="G6">
-        <v>-104.812639</v>
+        <v>-105.076491</v>
       </c>
       <c r="H6">
-        <v>40.441882999999997</v>
+        <v>40.321511000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7">
-        <v>-104.597244</v>
+        <v>-105.07213299999999</v>
       </c>
       <c r="H7">
-        <v>40.421965999999998</v>
+        <v>40.596778</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8">
-        <v>-104.575237</v>
+        <v>-105.00755599999999</v>
       </c>
       <c r="H8">
-        <v>40.419888999999998</v>
-      </c>
-      <c r="I8">
-        <v>-104.972905</v>
-      </c>
-      <c r="J8">
-        <v>39.742072999999998</v>
+        <v>40.565894999999998</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
       </c>
       <c r="G9">
-        <v>-105.07213299999999</v>
+        <v>-104.812639</v>
       </c>
       <c r="H9">
-        <v>40.596778</v>
+        <v>40.441882999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10">
+        <v>-104.597244</v>
+      </c>
+      <c r="H10">
+        <v>40.421965999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <v>-104.575237</v>
+      </c>
+      <c r="H11">
+        <v>40.419888999999998</v>
+      </c>
+      <c r="I11">
+        <v>-104.972905</v>
+      </c>
+      <c r="J11">
+        <v>39.742072999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12">
+        <v>-104.748876</v>
+      </c>
+      <c r="H12">
+        <v>40.422545999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
     <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
-    <hyperlink ref="E9" r:id="rId7"/>
-    <hyperlink ref="E3" r:id="rId8"/>
+    <hyperlink ref="E9" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
+    <hyperlink ref="E11" r:id="rId6"/>
+    <hyperlink ref="E3" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E4" r:id="rId9"/>
+    <hyperlink ref="E12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change marker image files to include size, issue #67
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
+++ b/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
@@ -553,7 +553,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,10 +622,10 @@
         <v>26</v>
       </c>
       <c r="G2">
-        <v>-105.082639</v>
+        <v>-105.083123</v>
       </c>
       <c r="H2">
-        <v>40.577306999999998</v>
+        <v>40.575507999999999</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -648,10 +648,10 @@
         <v>26</v>
       </c>
       <c r="G3">
-        <v>-105.019469</v>
+        <v>-105.019684</v>
       </c>
       <c r="H3">
-        <v>40.555596999999999</v>
+        <v>40.556147000000003</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -752,10 +752,10 @@
         <v>26</v>
       </c>
       <c r="G7">
-        <v>-105.07213299999999</v>
+        <v>-105.07219600000001</v>
       </c>
       <c r="H7">
-        <v>40.596778</v>
+        <v>40.596561999999999</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add news layers to education map, issue #75
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
+++ b/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
@@ -153,9 +153,6 @@
     <t>Focus on open source software and open data</t>
   </si>
   <si>
-    <t>LontitudeMain</t>
-  </si>
-  <si>
     <t>LatitudeMain</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>https://www.wgcd.org/conservation-education/</t>
+  </si>
+  <si>
+    <t>LongitudeMain</t>
   </si>
 </sst>
 </file>
@@ -596,10 +596,10 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
         <v>42</v>
-      </c>
-      <c r="J1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -630,19 +630,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -656,19 +656,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
       <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
@@ -682,19 +682,19 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
@@ -743,7 +743,7 @@
         <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>39</v>
@@ -870,19 +870,19 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Add initial major projects map, issue #139
Also add trail organizations and update various data.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
+++ b/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>This Excel workbook is an initial enventory of educational organizations that will be shown on the Basin Entities / Education - Organization map.</t>
   </si>
@@ -202,6 +202,21 @@
   </si>
   <si>
     <t>LongitudeMain</t>
+  </si>
+  <si>
+    <t>Fort Collins Museum of Discovery</t>
+  </si>
+  <si>
+    <t>Museum</t>
+  </si>
+  <si>
+    <t>Science museum</t>
+  </si>
+  <si>
+    <t>Hands on displays and programs</t>
+  </si>
+  <si>
+    <t>https://fcmod.org/</t>
   </si>
 </sst>
 </file>
@@ -550,10 +565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,33 +671,33 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
       </c>
       <c r="G4">
-        <v>-105.08512899999999</v>
+        <v>-105.07795</v>
       </c>
       <c r="H4">
-        <v>40.561815000000003</v>
+        <v>40.593600000000002</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -694,220 +709,247 @@
         <v>53</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
       <c r="G5">
-        <v>-104.71683400000001</v>
+        <v>-105.08512899999999</v>
       </c>
       <c r="H5">
-        <v>40.428258</v>
+        <v>40.561815000000003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
       </c>
       <c r="G6">
-        <v>-105.076491</v>
+        <v>-104.71683400000001</v>
       </c>
       <c r="H6">
-        <v>40.321511000000001</v>
+        <v>40.428258</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
       </c>
       <c r="G7">
-        <v>-105.07219600000001</v>
+        <v>-105.076491</v>
       </c>
       <c r="H7">
-        <v>40.596561999999999</v>
+        <v>40.321511000000001</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
       </c>
       <c r="G8">
-        <v>-105.00755599999999</v>
+        <v>-105.07219600000001</v>
       </c>
       <c r="H8">
-        <v>40.565894999999998</v>
+        <v>40.596561999999999</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
       </c>
       <c r="G9">
-        <v>-104.812639</v>
+        <v>-105.00755599999999</v>
       </c>
       <c r="H9">
-        <v>40.441882999999997</v>
+        <v>40.565894999999998</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10">
-        <v>-104.597244</v>
+        <v>-104.812639</v>
       </c>
       <c r="H10">
-        <v>40.421965999999998</v>
+        <v>40.441882999999997</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
       </c>
       <c r="G11">
-        <v>-104.575237</v>
+        <v>-104.597244</v>
       </c>
       <c r="H11">
-        <v>40.419888999999998</v>
-      </c>
-      <c r="I11">
-        <v>-104.972905</v>
-      </c>
-      <c r="J11">
-        <v>39.742072999999998</v>
+        <v>40.421965999999998</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <v>-104.575237</v>
+      </c>
+      <c r="H12">
+        <v>40.419888999999998</v>
+      </c>
+      <c r="I12">
+        <v>-104.972905</v>
+      </c>
+      <c r="J12">
+        <v>39.742072999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>26</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>-104.748876</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>40.422545999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
     <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E9" r:id="rId4"/>
-    <hyperlink ref="E10" r:id="rId5"/>
-    <hyperlink ref="E11" r:id="rId6"/>
+    <hyperlink ref="E10" r:id="rId4"/>
+    <hyperlink ref="E11" r:id="rId5"/>
+    <hyperlink ref="E12" r:id="rId6"/>
     <hyperlink ref="E3" r:id="rId7"/>
-    <hyperlink ref="E7" r:id="rId8"/>
-    <hyperlink ref="E4" r:id="rId9"/>
-    <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="E8" r:id="rId8"/>
+    <hyperlink ref="E5" r:id="rId9"/>
+    <hyperlink ref="E13" r:id="rId10"/>
+    <hyperlink ref="E4" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add East Troublesome wildfire soil burn severity, issue #159.
Also add many specific data items from various issues.
Turn on highlight for mouseover for various polygon layers.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
+++ b/workflow/BasinEntities/Education-Organizations/data/education-data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>This Excel workbook is an initial enventory of educational organizations that will be shown on the Basin Entities / Education - Organization map.</t>
   </si>
@@ -45,9 +45,6 @@
     <t>System tours, water conservation, teacher information.</t>
   </si>
   <si>
-    <t>https://www.northernwater.org/AboutUs/WaterEducation.aspx</t>
-  </si>
-  <si>
     <t>Poudre Heritage Alliance</t>
   </si>
   <si>
@@ -229,6 +226,48 @@
   </si>
   <si>
     <t>Annual Poudre River festival with exhibits.</t>
+  </si>
+  <si>
+    <t>The Water Desk</t>
+  </si>
+  <si>
+    <t>An initiative of the Center for Environmental Journalism at the University of Colorado Boulder</t>
+  </si>
+  <si>
+    <t>Journalism</t>
+  </si>
+  <si>
+    <t>https://waterdesk.org/</t>
+  </si>
+  <si>
+    <t>Fort Collins Water Works</t>
+  </si>
+  <si>
+    <t>Historical site.</t>
+  </si>
+  <si>
+    <t>http://poudrelandmarks.org/water-works</t>
+  </si>
+  <si>
+    <t>Water Resources Archive</t>
+  </si>
+  <si>
+    <t>Water resources archive</t>
+  </si>
+  <si>
+    <t>Historical documents related to water resources</t>
+  </si>
+  <si>
+    <t>https://lib.colostate.edu/find/archives-special-collections/collections/water-resources-archive/</t>
+  </si>
+  <si>
+    <t>https://www.northernwater.org/in-the-community/education-and-outreach</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Location is near New Belgium</t>
   </si>
 </sst>
 </file>
@@ -273,9 +312,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -577,10 +619,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <pane xSplit="3" ySplit="17" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,17 +640,18 @@
     <col min="8" max="8" width="13.21875" customWidth="1"/>
     <col min="9" max="9" width="15.5546875" customWidth="1"/>
     <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="11" max="11" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -614,39 +660,42 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>-105.083123</v>
@@ -655,24 +704,24 @@
         <v>40.575507999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>-105.019684</v>
@@ -681,24 +730,24 @@
         <v>40.556147000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <v>-105.07795</v>
@@ -707,287 +756,367 @@
         <v>40.593600000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>-105.14096000000001</v>
+      </c>
+      <c r="H5">
+        <v>40.615729999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
         <v>51</v>
       </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>-105.08512899999999</v>
+      </c>
+      <c r="H6">
+        <v>40.561815000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>54</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5">
-        <v>-105.08512899999999</v>
-      </c>
-      <c r="H5">
-        <v>40.561815000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6">
-        <v>-104.71683400000001</v>
-      </c>
-      <c r="H6">
-        <v>40.428258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>-104.71683400000001</v>
+      </c>
+      <c r="H7">
+        <v>40.428258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>-105.076491</v>
+      </c>
+      <c r="H8">
+        <v>40.321511000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>-105.07219600000001</v>
+      </c>
+      <c r="H9">
+        <v>40.596561999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7">
-        <v>-105.076491</v>
-      </c>
-      <c r="H7">
-        <v>40.321511000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8">
-        <v>-105.07219600000001</v>
-      </c>
-      <c r="H8">
-        <v>40.596561999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9">
-        <v>-105.00755599999999</v>
-      </c>
-      <c r="H9">
-        <v>40.565894999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>-105.00755599999999</v>
+      </c>
+      <c r="H10">
+        <v>40.565894999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>-104.812639</v>
+      </c>
+      <c r="H11">
+        <v>40.441882999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <v>-105.06962</v>
+      </c>
+      <c r="H12">
+        <v>40.592640000000003</v>
+      </c>
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>16</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10">
-        <v>-104.812639</v>
-      </c>
-      <c r="H10">
-        <v>40.441882999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11">
-        <v>-105.06962</v>
-      </c>
-      <c r="H11">
-        <v>40.592640000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12">
-        <v>-104.597244</v>
-      </c>
-      <c r="H12">
-        <v>40.421965999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13">
-        <v>-104.575237</v>
+        <v>-104.597244</v>
       </c>
       <c r="H13">
-        <v>40.419888999999998</v>
-      </c>
-      <c r="I13">
-        <v>-104.972905</v>
-      </c>
-      <c r="J13">
-        <v>39.742072999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>40.421965999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
         <v>26</v>
       </c>
       <c r="G14">
+        <v>-104.5198</v>
+      </c>
+      <c r="H14">
+        <v>40.491869999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>-104.575237</v>
+      </c>
+      <c r="H15">
+        <v>40.419888999999998</v>
+      </c>
+      <c r="I15">
+        <v>-104.972905</v>
+      </c>
+      <c r="J15">
+        <v>39.742072999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16">
+        <v>-105.08441000000001</v>
+      </c>
+      <c r="H16">
+        <v>40.572890000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17">
         <v>-104.748876</v>
       </c>
-      <c r="H14">
+      <c r="H17">
         <v>40.422545999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="E9" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E10" r:id="rId4"/>
-    <hyperlink ref="E12" r:id="rId5"/>
-    <hyperlink ref="E13" r:id="rId6"/>
-    <hyperlink ref="E3" r:id="rId7"/>
-    <hyperlink ref="E8" r:id="rId8"/>
-    <hyperlink ref="E5" r:id="rId9"/>
-    <hyperlink ref="E14" r:id="rId10"/>
-    <hyperlink ref="E4" r:id="rId11"/>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E11" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="E15" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E6" r:id="rId8"/>
+    <hyperlink ref="E17" r:id="rId9"/>
+    <hyperlink ref="E4" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>